<commit_message>
big commit of changes
</commit_message>
<xml_diff>
--- a/clockshift/4shot_metadata_file.xlsx
+++ b/clockshift/4shot_metadata_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Analysis Scripts\analysis\clockshift\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\UNOBTAINIUM\E_Carmen_Santiago\Analysis Scripts\analysis\clockshift\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -456,8 +456,8 @@
   </sheetPr>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add sinc^2 fit fcn with set bg
</commit_message>
<xml_diff>
--- a/clockshift/4shot_metadata_file.xlsx
+++ b/clockshift/4shot_metadata_file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
   <si>
     <t>filename</t>
   </si>
@@ -318,6 +318,18 @@
   </si>
   <si>
     <t>Half N</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>Total N for very cold</t>
+  </si>
+  <si>
+    <t>Total N for relatively hot</t>
+  </si>
+  <si>
+    <t>ToTF bound</t>
   </si>
 </sst>
 </file>
@@ -661,8 +673,8 @@
   </sheetPr>
   <dimension ref="A1:AP34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +688,7 @@
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.28515625" customWidth="1"/>
     <col min="20" max="25" width="10.85546875" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -3882,8 +3894,14 @@
         <f>Q31/U30</f>
         <v>20547.56143389679</v>
       </c>
+      <c r="U32" t="s">
+        <v>98</v>
+      </c>
+      <c r="V32" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="33" spans="16:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="16:22" x14ac:dyDescent="0.25">
       <c r="P33" t="s">
         <v>97</v>
       </c>
@@ -3891,11 +3909,39 @@
         <f>(6*T29/2)^(1/3) *U30*377</f>
         <v>1.7208801128830749E-30</v>
       </c>
+      <c r="S33" t="s">
+        <v>99</v>
+      </c>
+      <c r="T33">
+        <f>AVERAGEIFS(T2:T26,V2:V26,"&lt;&gt;",V2:V26,"&lt;"&amp;V33)</f>
+        <v>13307</v>
+      </c>
+      <c r="U33">
+        <f>(6*T33/2)^(1/3)*377</f>
+        <v>12884.725008242893</v>
+      </c>
+      <c r="V33">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="34" spans="16:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="16:22" x14ac:dyDescent="0.25">
       <c r="Q34" s="3">
         <f>Q33/U30</f>
         <v>16308.610317774486</v>
+      </c>
+      <c r="S34" t="s">
+        <v>100</v>
+      </c>
+      <c r="T34">
+        <f>AVERAGEIFS(T3:T27,V3:V27,"&lt;&gt;",V3:V27,"&gt;"&amp;V34)</f>
+        <v>35191.666666666664</v>
+      </c>
+      <c r="U34">
+        <f>(6*T34/2)^(1/3)*377</f>
+        <v>17818.113193982197</v>
+      </c>
+      <c r="V34">
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>